<commit_message>
ajustar tamaño de ventana y valores iniciales del slider en ContadorApp; restablecer valores después de revisar y traducir
</commit_message>
<xml_diff>
--- a/REVs/REV-11-03-2025.xlsx
+++ b/REVs/REV-11-03-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,20 +648,255 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>6VA35665</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B.BELLIES CLIP DUNCAN BEAR 8,5CM</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6VA27994</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>INVISIBOBBLE SPRUNCHIE DUO BRITISH ROYAL LADIES</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6VA32949</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>INVISIBOBBLE SPRUNCHIE DUO ITS SWEATER TIME</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>6VA14310</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GUYLOND LIMA UÑAS GRANDES 4 DISEÑOS</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>6VA14310</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GUYLOND LIMA UÑAS GRANDES 4 DISEÑOS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
agregar funcionalidad para restablecer el tamaño de la ventana al hacer doble clic en la barra de estado y aislado version desarrollo id en Titulo Ventana
</commit_message>
<xml_diff>
--- a/REVs/REV-11-03-2025.xlsx
+++ b/REVs/REV-11-03-2025.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +412,33 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="51.140625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="9.28515625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="23.7109375" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="8.42578125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="11.7109375" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="19.5703125" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="19.7109375" bestFit="1" customWidth="1" min="10" max="10"/>
+    <col width="13.42578125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="18.28515625" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="14.85546875" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="20" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="12.85546875" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="17.7109375" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="14.28515625" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="19.42578125" bestFit="1" customWidth="1" min="18" max="18"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -845,12 +864,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6VA14310</t>
+          <t>6VA40488</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>GUYLOND LIMA UÑAS GRANDES 4 DISEÑOS</t>
+          <t>MOSTROPI SET BOLIGRAFOS COLORES</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -875,28 +894,702 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6VA35401</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>INVOGUE HAPPY HOUR PESTAÑAS POSTIZAS MULTIPACK</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>6VA29059</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>HELLO BAGS BOLSA COSMETICOS IT-S ALL ABOUT BLANCO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>6VA29040</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>HELLO BAGS BOLSO MONEDERO MODELO ITS ALL ABOUT NEG</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6VA29044</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>HELLO BAGS BOLSO MONEDERO MODELO NO MIRES BLANCO</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>6VA29061</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>HELLO BAGS BOLSA COSMETICOS NEVER STOP BLANCO</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>6VA29045</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>HELLO BAGS BOLSO MONEDERO MODELO NO MIRES NEGRO</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>6VA19732</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>MOI RIÑONERA IMPERMEABLE VERDE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Pochete Bolsa Impermeável | 1und</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Pochete impermeável, perfeita para a praia, esportes 
+aquáticos e/ou ao ar livre.
+Bolsa estanque com alça adaptável para a cintura. Protege 
+teus pertences da água, areia ou pó. Zipper de triplo fecho 
+para maior segurança. Inclui uma aba de fecho do tipo 
+velcro.</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>MATERIAL: PVC
+MEDIDAS: 22.5x25.5cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>6VA19731</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>MOI RIÑONERA IMPERMEABLE ROSA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Pochete Bolsa Impermeável | 1und</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Pochete impermeável, perfeita para a praia, esportes 
+aquáticos e/ou ao ar livre.
+Bolsa estanque com alça adaptável para a cintura. Protege 
+teus pertences da água, areia ou pó. Zipper de triplo fecho 
+para maior segurança. Inclui uma aba de fecho do tipo 
+velcro.</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>MATERIAL: PVC
+MEDIDAS: 22.5x25.5cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>6VA19730</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>MOI RIÑONERA IMPERMEABLE TRANSPARENTE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Pochete Bolsa Impermeável | 1und</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Pochete impermeável, perfeita para a praia, esportes 
+aquáticos e/ou ao ar livre.
+Bolsa estanque com alça adaptável para a cintura. Protege 
+teus pertences da água, areia ou pó. Zipper de triplo fecho 
+para maior segurança. Inclui uma aba de fecho do tipo 
+velcro.</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>MATERIAL: PVC
+MEDIDAS: 22.5x25.5cm</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0TO01817</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BIOTHERM MEN SET FORCE SUPREME 75ML</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>6VA18358</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>W-7 BROW MASTER STENCIAL KIT</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>UND</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Regalo ZZ</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>afdafda</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>adwda</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Regalo ZZ</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
agregar funcionalidad para verificar el estado de revisión de productos y restablecer el tamaño de la ventana al hacer doble clic en la barra de estado
</commit_message>
<xml_diff>
--- a/REVs/REV-11-03-2025.xlsx
+++ b/REVs/REV-11-03-2025.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1576,20 +1576,67 @@
           <t>GR</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="inlineStr"/>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
-      <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
-      <c r="R22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>6VA18358</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>W-7 BROW MASTER STENCIAL KIT</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
actualizar base de datos y archivo REV-11-03-2025.xlsx
</commit_message>
<xml_diff>
--- a/REVs/REV-11-03-2025.xlsx
+++ b/REVs/REV-11-03-2025.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -1623,20 +1623,1553 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr"/>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
-      <c r="P23" t="inlineStr"/>
-      <c r="Q23" t="inlineStr"/>
-      <c r="R23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0TF26835</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>I-AM UNAU BAKUCHIOL VANILLA REWID MASK</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>No Tiene ES - TRADUCIDO</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Maschera Viso |Restauratrice| 27ml</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>Effetto: Aiuta a schiarire la pelle e migliora le rughe del 
+viso.
+Dopo aver deterso il viso, uniforma la texture della pelle 
+con un tonico e applica la maschera sul viso. Lascia agire 
+per 15-20 minuti, rimuovi la maschera e massaggia l'essenza 
+residua.</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Solo per uso esterno. Conservare in un luogo fresco e 
+asciutto.</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0TN03640</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MONSTER HIGH CLAWDEEN WOLF HAND CREAM</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ZMC00919</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>INSECT MATON 600 SP CASA Y JARDIN</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>600</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>3AF01720</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ENERGY FEELS ALWAYS LOVE EDT 28ML</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>PTESTE</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>PTESTE</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>PTESTE</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>PTESTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>6VA40635</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>HELLO KITTY LIP BALM 7G BALL 3D</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3AF01721</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ENERGY FEELS PARTY HARD EDT 28ML</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>3AF01719</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>ENERGY FEELS LIVE BRIGHT EDT 28ML</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2CA06584</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>ECO STYLE OLIVE OIL GEL 236 ML + 50% GRATIS</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0TP03790</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>MY PRIDE SET BROCHAS</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>6VA38727</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BILLY BROWN TIES EXECUTIVE SOCKS  36-40 M</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>6VA38734</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BILLY BROWN APEROL ITALIAN SOCKS  41-46 H</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>6VA35313</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>INVISIBOBBLE HAIRHALO MARGARITA BONITA</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE PT TITULO</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE PT USO</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE PT ADVERTENCIAS</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE PT +INFO</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE IT TITULO</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE IT USO</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE IT ADVERTENCIAS</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>MASTER TESTE IT +INFO</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>0TP03782</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>W-7 LIP CARE KIT - VANILLA</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>0TP03780</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>W-7 LIP CARE KIT - CHERRY</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>1DT00927</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>THE FRUIT COMPANY PASTA DENTAL MELON 60GR</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>1DT00926</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>THE FRUIT COMPANY PASTA DENTAL SANDIA 60GR</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1DT00929</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>THE FRUIT COMPANY PASTA DENTAL MELOCOTON 60GR</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>3AF01926</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>SJP LOVELY LOVELY LIGHTS BODY MIST 236ML</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>236</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>3AF01938</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TAI &amp; JON BODYMIST DOLCE ICE CREAM 250ML</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>3AF01940</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TAI &amp; JON BODYMIST FRUIT TRANQUILITY 250ML</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>250</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>6XS18308</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CERAVE CREMA HIDRATANTE REFILL 454GRS</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>454</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>6XS18295</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CERAVE LOCION HIDRATANTE REFILL 473ML</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>473</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>6XS18293</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CERAVE GEL LIMPIADOR ESPUMOSO REFILL 473ML</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>473</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>6XS18294</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CERAVE LIMPIADORA HIDRATANTE REFILL 473ML</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>473</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2LT03571</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>MET EXPOSITOR GOTAS BRONCEADORAS</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>LOTE</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>"8445984023355"</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>0MR27448</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>MET BRONZE DROPS GOTAS BRONCEADORAS 30ML</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2LT03460</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TECHNIC LOTE JELLY BLUSH - PINK BURST</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>LOTE</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>"5021769247371"</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>0MR27166</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TECHNIC JELLY BLUSH - PINK BURST</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>teste sku</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>teste titulo</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>teste1</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
agregar archivo todo.txt con tareas pendientes y notas sobre mejoras en la funcionalidad de revisión y búsqueda en la base de datos
</commit_message>
<xml_diff>
--- a/REVs/REV-11-03-2025.xlsx
+++ b/REVs/REV-11-03-2025.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R53"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -3124,7 +3124,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
           <t>Revisado y Traducido</t>
@@ -3170,6 +3169,156 @@
           <t>teste1</t>
         </is>
       </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>0TS04033</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>BABARIA SUN FACIAL CREMA MOSQUETON SPF50+ 50ML</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>0TS04035</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>BABARIA SUN LECHE SOLAR SPF30+ 100ML</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>0TS04032</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>BABARIA SUN FACIAL BRUMA PROTECT. SPF50+ 75ML</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Consumo</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
+      <c r="Q56" t="inlineStr"/>
+      <c r="R56" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>